<commit_message>
Working input from WinForm to Excel table
</commit_message>
<xml_diff>
--- a/Sihter/input/SihtericaIN.xlsx
+++ b/Sihter/input/SihtericaIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maram\source\repos\Sihter\Sihter\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5D8C3F-4CFF-494C-8503-E8D2078FC6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BD2067-A810-4679-A689-63792F64F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8B90615D-394E-486E-9C39-3590B30B6731}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AJ$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AJ$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>Dom zdravlja bjelovarsko-bilogorske županije</t>
   </si>
@@ -236,20 +236,23 @@
     <t>U &lt;mjestu&gt; , dana &lt;datum&gt; &lt;godina&gt;.</t>
   </si>
   <si>
-    <t>&lt;mjesec&gt; &lt;godina&gt;</t>
-  </si>
-  <si>
     <t>&lt;radnik&gt;</t>
   </si>
   <si>
     <t>&lt;org.jed&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mjesec&gt;</t>
+  </si>
+  <si>
+    <t>&lt;godina&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +311,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -422,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -457,6 +466,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -517,12 +528,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -545,19 +550,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,26 +957,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ64"/>
+  <dimension ref="A1:AM63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="5" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="19.85546875" style="2" customWidth="1"/>
-    <col min="5" max="13" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="2" customWidth="1"/>
+    <col min="5" max="35" width="5" style="2" customWidth="1"/>
     <col min="36" max="36" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="2"/>
+    <col min="37" max="16384" width="5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -996,7 +995,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S1" s="47"/>
       <c r="T1" s="47"/>
@@ -1017,54 +1016,56 @@
       <c r="AI1" s="47"/>
       <c r="AJ1" s="47"/>
     </row>
-    <row r="2" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="50"/>
-      <c r="Z3" s="50"/>
-      <c r="AA3" s="50"/>
-      <c r="AB3" s="50"/>
-      <c r="AC3" s="50"/>
-      <c r="AD3" s="50"/>
-      <c r="AE3" s="50"/>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="50"/>
-      <c r="AH3" s="50"/>
-      <c r="AI3" s="50"/>
-      <c r="AJ3" s="51"/>
-    </row>
-    <row r="4" spans="1:36" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="49"/>
+    </row>
+    <row r="4" spans="1:39" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1075,104 +1076,104 @@
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="18">
         <v>1</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="18">
         <v>2</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="18">
         <v>3</v>
       </c>
-      <c r="H4" s="52">
+      <c r="H4" s="18">
         <v>4</v>
       </c>
-      <c r="I4" s="52">
+      <c r="I4" s="18">
         <v>5</v>
       </c>
-      <c r="J4" s="52">
+      <c r="J4" s="18">
         <v>6</v>
       </c>
-      <c r="K4" s="52">
+      <c r="K4" s="18">
         <v>7</v>
       </c>
-      <c r="L4" s="52">
+      <c r="L4" s="18">
         <v>8</v>
       </c>
-      <c r="M4" s="52">
+      <c r="M4" s="18">
         <v>9</v>
       </c>
-      <c r="N4" s="52">
+      <c r="N4" s="18">
         <v>10</v>
       </c>
-      <c r="O4" s="52">
+      <c r="O4" s="18">
         <v>11</v>
       </c>
-      <c r="P4" s="52">
+      <c r="P4" s="18">
         <v>12</v>
       </c>
-      <c r="Q4" s="52">
+      <c r="Q4" s="18">
         <v>13</v>
       </c>
-      <c r="R4" s="52">
+      <c r="R4" s="18">
         <v>14</v>
       </c>
-      <c r="S4" s="52">
+      <c r="S4" s="18">
         <v>15</v>
       </c>
-      <c r="T4" s="52">
+      <c r="T4" s="18">
         <v>16</v>
       </c>
-      <c r="U4" s="52">
+      <c r="U4" s="18">
         <v>17</v>
       </c>
-      <c r="V4" s="52">
+      <c r="V4" s="18">
         <v>18</v>
       </c>
-      <c r="W4" s="52">
+      <c r="W4" s="18">
         <v>19</v>
       </c>
-      <c r="X4" s="52">
+      <c r="X4" s="18">
         <v>20</v>
       </c>
-      <c r="Y4" s="52">
+      <c r="Y4" s="18">
         <v>21</v>
       </c>
-      <c r="Z4" s="52">
+      <c r="Z4" s="18">
         <v>22</v>
       </c>
-      <c r="AA4" s="52">
+      <c r="AA4" s="18">
         <v>23</v>
       </c>
-      <c r="AB4" s="52">
+      <c r="AB4" s="18">
         <v>24</v>
       </c>
-      <c r="AC4" s="52">
+      <c r="AC4" s="18">
         <v>25</v>
       </c>
-      <c r="AD4" s="52">
+      <c r="AD4" s="18">
         <v>26</v>
       </c>
-      <c r="AE4" s="52">
+      <c r="AE4" s="18">
         <v>27</v>
       </c>
-      <c r="AF4" s="52">
+      <c r="AF4" s="18">
         <v>28</v>
       </c>
-      <c r="AG4" s="52">
+      <c r="AG4" s="18">
         <v>29</v>
       </c>
-      <c r="AH4" s="52">
+      <c r="AH4" s="18">
         <v>30</v>
       </c>
-      <c r="AI4" s="52">
+      <c r="AI4" s="18">
         <v>31</v>
       </c>
       <c r="AJ4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -1210,15 +1211,15 @@
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6"/>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1251,16 +1252,17 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="6"/>
-    </row>
-    <row r="7" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AM6" s="19"/>
+    </row>
+    <row r="7" spans="1:39" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1294,56 +1296,152 @@
       <c r="AI7" s="6"/>
       <c r="AJ7" s="6"/>
     </row>
-    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6"/>
-      <c r="AJ8" s="6"/>
-    </row>
-    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="6" t="str">
+        <f xml:space="preserve"> IF((E7 - E6) &lt;&gt; 0, E7 - E6, "")</f>
+        <v/>
+      </c>
+      <c r="F8" s="6" t="str">
+        <f t="shared" ref="F8:AI8" si="0" xml:space="preserve"> IF((F7 - F6) &lt;&gt; 0, F7 - F6, "")</f>
+        <v/>
+      </c>
+      <c r="G8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="O8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="R8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="T8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="U8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="V8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="W8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="X8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Y8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AA8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AC8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AD8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AE8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AF8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AH8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AI8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AJ8" s="6" t="str">
+        <f t="shared" ref="AJ7:AJ34" si="1">IF(SUM(E8:AI8)&gt;0, SUM(E8:AI8), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="28">
         <v>4</v>
       </c>
       <c r="B9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="39" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="43"/>
@@ -1378,12 +1476,15 @@
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
-      <c r="AJ9" s="6"/>
-    </row>
-    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
+      <c r="AJ9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
       <c r="B10" s="46"/>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="39" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="43"/>
@@ -1414,12 +1515,15 @@
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-    </row>
-    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
+      <c r="AJ10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
       <c r="B11" s="46"/>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="39" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="43"/>
@@ -1454,12 +1558,15 @@
       <c r="AG11" s="6"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
-      <c r="AJ11" s="6"/>
-    </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
+      <c r="AJ11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
       <c r="B12" s="46"/>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="39" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="43"/>
@@ -1494,12 +1601,15 @@
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
-      <c r="AJ12" s="6"/>
-    </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
+      <c r="AJ12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
       <c r="B13" s="46"/>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="39" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="43"/>
@@ -1534,12 +1644,15 @@
       <c r="AG13" s="6"/>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
-    </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
+      <c r="AJ13" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
       <c r="B14" s="46"/>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="39" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="43"/>
@@ -1574,12 +1687,15 @@
       <c r="AG14" s="6"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
-      <c r="AJ14" s="6"/>
-    </row>
-    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
+      <c r="AJ14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
       <c r="B15" s="46"/>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="39" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="43"/>
@@ -1614,12 +1730,15 @@
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
-      <c r="AJ15" s="6"/>
-    </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
+      <c r="AJ15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
       <c r="B16" s="46"/>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="39" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="43"/>
@@ -1654,12 +1773,15 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
+      <c r="AJ16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="46"/>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="39" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="43"/>
@@ -1694,12 +1816,15 @@
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
-      <c r="AJ17" s="6"/>
+      <c r="AJ17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="46"/>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="43"/>
@@ -1734,12 +1859,15 @@
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
+      <c r="AJ18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="46"/>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="43"/>
@@ -1774,12 +1902,15 @@
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
+      <c r="AJ19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="46"/>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="39" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="43"/>
@@ -1814,12 +1945,15 @@
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
+      <c r="AJ20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="46"/>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="43"/>
@@ -1854,12 +1988,15 @@
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
+      <c r="AJ21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="39" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="43"/>
@@ -1894,12 +2031,15 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
+      <c r="AJ22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="46"/>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="39" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="43"/>
@@ -1934,12 +2074,15 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
+      <c r="AJ23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="46"/>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="39" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="43"/>
@@ -1974,12 +2117,15 @@
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
       <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
+      <c r="AJ24" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="46"/>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="39" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="43"/>
@@ -2014,15 +2160,18 @@
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
-      <c r="AJ25" s="6"/>
+      <c r="AJ25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="46"/>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="37"/>
+      <c r="D26" s="39"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2054,19 +2203,22 @@
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
-      <c r="AJ26" s="6"/>
+      <c r="AJ26" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="26">
+      <c r="A27" s="28">
         <v>5</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="37"/>
+      <c r="D27" s="39"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -2098,15 +2250,18 @@
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
-      <c r="AJ27" s="6"/>
+      <c r="AJ27" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="44"/>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="37"/>
+      <c r="D28" s="39"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -2138,15 +2293,18 @@
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
-      <c r="AJ28" s="6"/>
+      <c r="AJ28" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="44"/>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -2178,15 +2336,18 @@
       <c r="AG29" s="6"/>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
-      <c r="AJ29" s="6"/>
+      <c r="AJ29" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="44"/>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="37"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -2218,15 +2379,18 @@
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
       <c r="AI30" s="6"/>
-      <c r="AJ30" s="6"/>
+      <c r="AJ30" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="44"/>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="37"/>
+      <c r="D31" s="39"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -2258,15 +2422,18 @@
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
       <c r="AI31" s="6"/>
-      <c r="AJ31" s="6"/>
+      <c r="AJ31" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="44"/>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="37"/>
+      <c r="D32" s="39"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -2298,13 +2465,20 @@
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
       <c r="AI32" s="6"/>
-      <c r="AJ32" s="6"/>
+      <c r="AJ32" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="39"/>
+      <c r="A33" s="6">
+        <v>6</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -2336,14 +2510,17 @@
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
       <c r="AI33" s="6"/>
-      <c r="AJ33" s="6"/>
+      <c r="AJ33" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" s="41"/>
       <c r="D34" s="42"/>
@@ -2378,14 +2555,17 @@
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
-      <c r="AJ34" s="6"/>
+      <c r="AJ34" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="42"/>
@@ -2420,165 +2600,171 @@
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
       <c r="AI35" s="6"/>
-      <c r="AJ35" s="6"/>
-    </row>
-    <row r="36" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
+      <c r="AJ35" s="6" t="str">
+        <f>IF(SUM(E35:AI35)&gt;0, SUM(E35:AI35), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12">
+        <v>2</v>
+      </c>
+      <c r="G36" s="12">
+        <v>3</v>
+      </c>
+      <c r="H36" s="12">
+        <v>4</v>
+      </c>
+      <c r="I36" s="12">
+        <v>5</v>
+      </c>
+      <c r="J36" s="12">
+        <v>6</v>
+      </c>
+      <c r="K36" s="12">
+        <v>7</v>
+      </c>
+      <c r="L36" s="12">
         <v>8</v>
       </c>
-      <c r="B36" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-      <c r="AF36" s="6"/>
-      <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
-      <c r="AI36" s="6"/>
-      <c r="AJ36" s="6"/>
-    </row>
-    <row r="37" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="12">
-        <v>1</v>
-      </c>
-      <c r="F37" s="12">
-        <v>2</v>
-      </c>
-      <c r="G37" s="12">
-        <v>3</v>
-      </c>
-      <c r="H37" s="12">
-        <v>4</v>
-      </c>
-      <c r="I37" s="12">
+      <c r="M36" s="12">
+        <v>9</v>
+      </c>
+      <c r="N36" s="12">
+        <v>10</v>
+      </c>
+      <c r="O36" s="12">
+        <v>11</v>
+      </c>
+      <c r="P36" s="12">
+        <v>12</v>
+      </c>
+      <c r="Q36" s="12">
+        <v>13</v>
+      </c>
+      <c r="R36" s="12">
+        <v>14</v>
+      </c>
+      <c r="S36" s="12">
+        <v>15</v>
+      </c>
+      <c r="T36" s="12">
+        <v>16</v>
+      </c>
+      <c r="U36" s="12">
+        <v>17</v>
+      </c>
+      <c r="V36" s="12">
+        <v>18</v>
+      </c>
+      <c r="W36" s="12">
+        <v>19</v>
+      </c>
+      <c r="X36" s="12">
+        <v>20</v>
+      </c>
+      <c r="Y36" s="12">
+        <v>21</v>
+      </c>
+      <c r="Z36" s="12">
+        <v>22</v>
+      </c>
+      <c r="AA36" s="12">
+        <v>23</v>
+      </c>
+      <c r="AB36" s="12">
+        <v>24</v>
+      </c>
+      <c r="AC36" s="12">
+        <v>25</v>
+      </c>
+      <c r="AD36" s="12">
+        <v>26</v>
+      </c>
+      <c r="AE36" s="12">
+        <v>27</v>
+      </c>
+      <c r="AF36" s="12">
+        <v>28</v>
+      </c>
+      <c r="AG36" s="12">
+        <v>29</v>
+      </c>
+      <c r="AH36" s="12">
+        <v>30</v>
+      </c>
+      <c r="AI36" s="12">
+        <v>31</v>
+      </c>
+      <c r="AJ36" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J37" s="12">
-        <v>6</v>
-      </c>
-      <c r="K37" s="12">
-        <v>7</v>
-      </c>
-      <c r="L37" s="12">
-        <v>8</v>
-      </c>
-      <c r="M37" s="12">
+    </row>
+    <row r="37" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12">
         <v>9</v>
       </c>
-      <c r="N37" s="12">
+      <c r="B37" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+      <c r="AA37" s="6"/>
+      <c r="AB37" s="6"/>
+      <c r="AC37" s="6"/>
+      <c r="AD37" s="6"/>
+      <c r="AE37" s="6"/>
+      <c r="AF37" s="6"/>
+      <c r="AG37" s="6"/>
+      <c r="AH37" s="6"/>
+      <c r="AI37" s="6"/>
+      <c r="AJ37" s="6" t="str">
+        <f t="shared" ref="AJ37:AJ56" si="2">IF(SUM(E37:AI37)&gt;0, SUM(E37:AI37), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
         <v>10</v>
       </c>
-      <c r="O37" s="12">
-        <v>11</v>
-      </c>
-      <c r="P37" s="12">
-        <v>12</v>
-      </c>
-      <c r="Q37" s="12">
-        <v>13</v>
-      </c>
-      <c r="R37" s="12">
-        <v>14</v>
-      </c>
-      <c r="S37" s="12">
-        <v>15</v>
-      </c>
-      <c r="T37" s="12">
-        <v>16</v>
-      </c>
-      <c r="U37" s="12">
-        <v>17</v>
-      </c>
-      <c r="V37" s="12">
-        <v>18</v>
-      </c>
-      <c r="W37" s="12">
-        <v>19</v>
-      </c>
-      <c r="X37" s="12">
-        <v>20</v>
-      </c>
-      <c r="Y37" s="12">
-        <v>21</v>
-      </c>
-      <c r="Z37" s="12">
-        <v>22</v>
-      </c>
-      <c r="AA37" s="12">
-        <v>23</v>
-      </c>
-      <c r="AB37" s="12">
-        <v>24</v>
-      </c>
-      <c r="AC37" s="12">
-        <v>25</v>
-      </c>
-      <c r="AD37" s="12">
-        <v>26</v>
-      </c>
-      <c r="AE37" s="12">
-        <v>27</v>
-      </c>
-      <c r="AF37" s="12">
-        <v>28</v>
-      </c>
-      <c r="AG37" s="12">
-        <v>29</v>
-      </c>
-      <c r="AH37" s="12">
-        <v>30</v>
-      </c>
-      <c r="AI37" s="12">
-        <v>31</v>
-      </c>
-      <c r="AJ37" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12">
-        <v>9</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="B38" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -2610,17 +2796,20 @@
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
       <c r="AI38" s="6"/>
-      <c r="AJ38" s="6"/>
+      <c r="AJ38" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:36" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <v>10</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
+        <v>11</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -2652,17 +2841,20 @@
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
       <c r="AI39" s="6"/>
-      <c r="AJ39" s="6"/>
+      <c r="AJ39" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:36" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <v>11</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -2694,17 +2886,20 @@
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
       <c r="AI40" s="6"/>
-      <c r="AJ40" s="6"/>
+      <c r="AJ40" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
-        <v>12</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
+      <c r="A41" s="28">
+        <v>13</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
@@ -2736,17 +2931,18 @@
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
       <c r="AI41" s="6"/>
-      <c r="AJ41" s="6"/>
-    </row>
-    <row r="42" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="26">
-        <v>13</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
+      <c r="AJ41" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="29"/>
+      <c r="B42" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -2778,15 +2974,18 @@
       <c r="AG42" s="6"/>
       <c r="AH42" s="6"/>
       <c r="AI42" s="6"/>
-      <c r="AJ42" s="6"/>
-    </row>
-    <row r="43" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27"/>
-      <c r="B43" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
+      <c r="AJ42" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:36" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="30"/>
+      <c r="B43" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="27"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -2818,15 +3017,20 @@
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
       <c r="AI43" s="6"/>
-      <c r="AJ43" s="6"/>
+      <c r="AJ43" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="44" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="28"/>
-      <c r="B44" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="25"/>
+      <c r="A44" s="28">
+        <v>14</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="26"/>
+      <c r="D44" s="27"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -2858,17 +3062,18 @@
       <c r="AG44" s="6"/>
       <c r="AH44" s="6"/>
       <c r="AI44" s="6"/>
-      <c r="AJ44" s="6"/>
+      <c r="AJ44" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="26">
-        <v>14</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="25"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2900,15 +3105,18 @@
       <c r="AG45" s="6"/>
       <c r="AH45" s="6"/>
       <c r="AI45" s="6"/>
-      <c r="AJ45" s="6"/>
+      <c r="AJ45" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="46" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="27"/>
-      <c r="B46" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="25"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="26"/>
+      <c r="D46" s="27"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -2940,15 +3148,20 @@
       <c r="AG46" s="6"/>
       <c r="AH46" s="6"/>
       <c r="AI46" s="6"/>
-      <c r="AJ46" s="6"/>
-    </row>
-    <row r="47" spans="1:36" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="28"/>
-      <c r="B47" s="23" t="s">
-        <v>47</v>
+      <c r="AJ46" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>15</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>48</v>
       </c>
       <c r="C47" s="24"/>
-      <c r="D47" s="25"/>
+      <c r="D47" s="24"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2980,17 +3193,20 @@
       <c r="AG47" s="6"/>
       <c r="AH47" s="6"/>
       <c r="AI47" s="6"/>
-      <c r="AJ47" s="6"/>
-    </row>
-    <row r="48" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ47" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:36" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
-        <v>15</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
+        <v>16</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -3022,17 +3238,20 @@
       <c r="AG48" s="6"/>
       <c r="AH48" s="6"/>
       <c r="AI48" s="6"/>
-      <c r="AJ48" s="6"/>
+      <c r="AJ48" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="49" spans="1:36" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
-        <v>16</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -3064,17 +3283,20 @@
       <c r="AG49" s="6"/>
       <c r="AH49" s="6"/>
       <c r="AI49" s="6"/>
-      <c r="AJ49" s="6"/>
-    </row>
-    <row r="50" spans="1:36" ht="15" x14ac:dyDescent="0.2">
+      <c r="AJ49" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:36" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
-        <v>17</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="26"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -3106,17 +3328,22 @@
       <c r="AG50" s="6"/>
       <c r="AH50" s="6"/>
       <c r="AI50" s="6"/>
-      <c r="AJ50" s="6"/>
-    </row>
-    <row r="51" spans="1:36" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
-        <v>18</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="25"/>
+      <c r="AJ50" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:36" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="28">
+        <v>19</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="34"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -3148,19 +3375,18 @@
       <c r="AG51" s="6"/>
       <c r="AH51" s="6"/>
       <c r="AI51" s="6"/>
-      <c r="AJ51" s="6"/>
-    </row>
-    <row r="52" spans="1:36" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="26">
-        <v>19</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="32"/>
+      <c r="AJ51" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="29"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="34"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -3192,15 +3418,18 @@
       <c r="AG52" s="6"/>
       <c r="AH52" s="6"/>
       <c r="AI52" s="6"/>
-      <c r="AJ52" s="6"/>
+      <c r="AJ52" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="53" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="27"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="32"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="34"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -3232,15 +3461,16 @@
       <c r="AG53" s="6"/>
       <c r="AH53" s="6"/>
       <c r="AI53" s="6"/>
-      <c r="AJ53" s="6"/>
-    </row>
-    <row r="54" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="32"/>
+      <c r="AJ53" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:36" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="29"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -3272,13 +3502,18 @@
       <c r="AG54" s="6"/>
       <c r="AH54" s="6"/>
       <c r="AI54" s="6"/>
-      <c r="AJ54" s="6"/>
-    </row>
-    <row r="55" spans="1:36" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="27"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
+      <c r="AJ54" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="29"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="34"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -3310,15 +3545,18 @@
       <c r="AG55" s="6"/>
       <c r="AH55" s="6"/>
       <c r="AI55" s="6"/>
-      <c r="AJ55" s="6"/>
-    </row>
-    <row r="56" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="27"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="32"/>
+      <c r="AJ55" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:36" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="30"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="34"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -3350,136 +3588,100 @@
       <c r="AG56" s="6"/>
       <c r="AH56" s="6"/>
       <c r="AI56" s="6"/>
-      <c r="AJ56" s="6"/>
-    </row>
-    <row r="57" spans="1:36" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="28"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="32"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
-      <c r="S57" s="6"/>
-      <c r="T57" s="6"/>
-      <c r="U57" s="6"/>
-      <c r="V57" s="6"/>
-      <c r="W57" s="6"/>
-      <c r="X57" s="6"/>
-      <c r="Y57" s="6"/>
-      <c r="Z57" s="6"/>
-      <c r="AA57" s="6"/>
-      <c r="AB57" s="6"/>
-      <c r="AC57" s="6"/>
-      <c r="AD57" s="6"/>
-      <c r="AE57" s="6"/>
-      <c r="AF57" s="6"/>
-      <c r="AG57" s="6"/>
-      <c r="AH57" s="6"/>
-      <c r="AI57" s="6"/>
-      <c r="AJ57" s="6"/>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="18"/>
-      <c r="P58" s="18"/>
-      <c r="Q58" s="18"/>
-      <c r="R58" s="18"/>
-      <c r="S58" s="18"/>
-      <c r="T58" s="18"/>
-      <c r="U58" s="18"/>
-      <c r="V58" s="18"/>
-      <c r="W58" s="18"/>
-      <c r="X58" s="18"/>
-      <c r="Y58" s="18"/>
-      <c r="Z58" s="18"/>
-      <c r="AA58" s="18"/>
-      <c r="AB58" s="18"/>
-      <c r="AC58" s="18"/>
-      <c r="AD58" s="18"/>
-      <c r="AE58" s="18"/>
-      <c r="AF58" s="18"/>
-      <c r="AG58" s="18"/>
-      <c r="AH58" s="18"/>
-      <c r="AI58" s="18"/>
-      <c r="AJ58" s="18"/>
-    </row>
-    <row r="59" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="19" t="s">
+      <c r="AJ56" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
+      <c r="P57" s="20"/>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="20"/>
+      <c r="T57" s="20"/>
+      <c r="U57" s="20"/>
+      <c r="V57" s="20"/>
+      <c r="W57" s="20"/>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="20"/>
+      <c r="Z57" s="20"/>
+      <c r="AA57" s="20"/>
+      <c r="AB57" s="20"/>
+      <c r="AC57" s="20"/>
+      <c r="AD57" s="20"/>
+      <c r="AE57" s="20"/>
+      <c r="AF57" s="20"/>
+      <c r="AG57" s="20"/>
+      <c r="AH57" s="20"/>
+      <c r="AI57" s="20"/>
+      <c r="AJ57" s="20"/>
+    </row>
+    <row r="58" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="AJ59" s="14"/>
-    </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="AJ58" s="14"/>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="P61" s="20" t="s">
+      <c r="P60" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Q61" s="21"/>
-      <c r="R61" s="21"/>
-      <c r="S61" s="21"/>
-      <c r="T61" s="21"/>
-      <c r="U61" s="21"/>
-      <c r="V61" s="21"/>
-      <c r="W61" s="21"/>
-      <c r="X61" s="21"/>
-      <c r="Y61" s="21"/>
-      <c r="Z61" s="21"/>
-      <c r="AA61" s="21"/>
-      <c r="AB61" s="21"/>
-      <c r="AC61" s="21"/>
-      <c r="AD61" s="21"/>
-      <c r="AE61" s="21"/>
-      <c r="AF61" s="21"/>
-      <c r="AG61" s="21"/>
-      <c r="AH61" s="14"/>
-      <c r="AI61" s="14"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="23"/>
+      <c r="S60" s="23"/>
+      <c r="T60" s="23"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="23"/>
+      <c r="W60" s="23"/>
+      <c r="X60" s="23"/>
+      <c r="Y60" s="23"/>
+      <c r="Z60" s="23"/>
+      <c r="AA60" s="23"/>
+      <c r="AB60" s="23"/>
+      <c r="AC60" s="23"/>
+      <c r="AD60" s="23"/>
+      <c r="AE60" s="23"/>
+      <c r="AF60" s="23"/>
+      <c r="AG60" s="23"/>
+      <c r="AH60" s="14"/>
+      <c r="AI60" s="14"/>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A62" s="17"/>
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
-    </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="66">
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="R1:AJ1"/>
-    <mergeCell ref="A3:L3"/>
     <mergeCell ref="M3:AJ3"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="A3:C3"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A9:A26"/>
     <mergeCell ref="B9:B26"/>
@@ -3500,51 +3702,50 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:D41"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B49:D49"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="A58:AJ58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="P61:AG61"/>
+    <mergeCell ref="A57:AJ57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="P60:AG60"/>
+    <mergeCell ref="B49:D49"/>
     <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="A52:A57"/>
-    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="A51:A56"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="36" max="35" man="1"/>
+    <brk id="35" max="35" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>